<commit_message>
Se actualizo la lista de componentes
</commit_message>
<xml_diff>
--- a/Componentes Disponibles/Stock Arturo Integrados.xlsx
+++ b/Componentes Disponibles/Stock Arturo Integrados.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Arturo UTN\UTN_Arturo\Componentes Disponibles\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="45" windowWidth="18855" windowHeight="8460"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8250"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -16,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="55">
   <si>
     <t>CA3086</t>
   </si>
@@ -178,13 +183,16 @@
   </si>
   <si>
     <t>BC327</t>
+  </si>
+  <si>
+    <t>Cantidad</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -201,7 +209,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -209,18 +217,42 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -267,7 +299,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -299,9 +331,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -333,6 +366,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -508,323 +542,459 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J38"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A4:J41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="A39" sqref="A39"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="D41" sqref="D41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5">
-      <c r="A1" t="s">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B4" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:5">
-      <c r="A2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3" t="s">
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B6" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4" t="s">
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B7" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="E4">
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
-      <c r="A5" t="s">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B8" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E5">
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
-      <c r="A6" t="s">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B9" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="7" spans="1:5">
-      <c r="A7" t="s">
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B10" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E7">
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
-      <c r="A8" t="s">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B11" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="E8">
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
-      <c r="A9" t="s">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B12" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E9">
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
-      <c r="A10" t="s">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B13" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="11" spans="1:5">
-      <c r="A11" t="s">
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B14" s="1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="12" spans="1:5">
-      <c r="A12" t="s">
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B15" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="13" spans="1:5">
-      <c r="A13" t="s">
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B16" s="1" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="14" spans="1:5">
-      <c r="A14" t="s">
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B17" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="15" spans="1:5">
-      <c r="A15" t="s">
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B18" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="E15">
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1">
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:10">
-      <c r="A17" t="s">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="18" spans="1:10">
-      <c r="B18" t="s">
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A21" s="1"/>
+      <c r="B21" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="H18" t="s">
+      <c r="C21" s="1"/>
+      <c r="D21" s="1">
+        <v>1</v>
+      </c>
+      <c r="H21" s="1" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="19" spans="1:10">
-      <c r="A19" t="s">
+      <c r="I21" s="1"/>
+      <c r="J21" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B22" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="H19" t="s">
+      <c r="C22" s="1"/>
+      <c r="D22" s="1">
+        <v>1</v>
+      </c>
+      <c r="H22" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="J19">
+      <c r="I22" s="1"/>
+      <c r="J22" s="1">
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="1:10">
-      <c r="A20">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A23" s="1">
         <v>152</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B23" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="D20">
+      <c r="C23" s="1"/>
+      <c r="D23" s="1">
         <v>4</v>
       </c>
-      <c r="H20" t="s">
+      <c r="H23" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="J20">
+      <c r="I23" s="1"/>
+      <c r="J23" s="1">
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:10">
-      <c r="A21">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A24" s="1">
         <v>104</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B24" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="D21">
+      <c r="C24" s="1"/>
+      <c r="D24" s="1">
         <v>2</v>
       </c>
-      <c r="H21" t="s">
+      <c r="H24" s="1" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="22" spans="1:10">
-      <c r="A22" t="s">
+      <c r="I24" s="1"/>
+      <c r="J24" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B25" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="H22" t="s">
+      <c r="C25" s="1"/>
+      <c r="D25" s="1">
+        <v>1</v>
+      </c>
+      <c r="H25" s="1" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="23" spans="1:10">
-      <c r="A23" t="s">
+      <c r="I25" s="1"/>
+      <c r="J25" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B26" s="1" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="24" spans="1:10">
-      <c r="A24">
+      <c r="C26" s="1"/>
+      <c r="D26" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A27" s="1">
         <v>103</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B27" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="D24">
+      <c r="C27" s="1"/>
+      <c r="D27" s="1">
         <v>3</v>
       </c>
     </row>
-    <row r="25" spans="1:10">
-      <c r="A25">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A28" s="1">
         <v>472</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B28" s="1" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="26" spans="1:10">
-      <c r="A26">
-        <v>1</v>
-      </c>
-      <c r="B26" t="s">
+      <c r="C28" s="1"/>
+      <c r="D28" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A29" s="1">
+        <v>1</v>
+      </c>
+      <c r="B29" s="1" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="27" spans="1:10">
-      <c r="A27" t="s">
+      <c r="C29" s="1"/>
+      <c r="D29" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B30" s="1" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="28" spans="1:10">
-      <c r="A28">
+      <c r="C30" s="1"/>
+      <c r="D30" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A31" s="1">
         <v>47</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B31" s="1" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="29" spans="1:10">
-      <c r="A29" t="s">
+      <c r="C31" s="1"/>
+      <c r="D31" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B32" s="1" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="30" spans="1:10">
-      <c r="A30">
+      <c r="C32" s="1"/>
+      <c r="D32" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="1">
         <v>100</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B33" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="D30">
+      <c r="C33" s="1"/>
+      <c r="D33" s="1">
         <v>3</v>
       </c>
     </row>
-    <row r="31" spans="1:10">
-      <c r="A31">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="1">
         <v>224</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B34" s="1" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="34" spans="1:3">
-      <c r="A34" t="s">
+      <c r="C34" s="1"/>
+      <c r="D34" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="36" spans="1:3">
-      <c r="A36" t="s">
+      <c r="B37" s="1"/>
+      <c r="C37" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="1"/>
+      <c r="B38" s="1"/>
+      <c r="C38" s="1"/>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="C36">
+      <c r="B39" s="1"/>
+      <c r="C39" s="1">
         <v>5</v>
       </c>
     </row>
-    <row r="37" spans="1:3">
-      <c r="A37" t="s">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="38" spans="1:3">
-      <c r="A38" t="s">
+      <c r="B40" s="1"/>
+      <c r="C40" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="C38">
+      <c r="B41" s="1"/>
+      <c r="C41" s="1">
         <v>7</v>
       </c>
     </row>
@@ -835,24 +1005,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Se actualizo el excel de componentes
</commit_message>
<xml_diff>
--- a/Componentes Disponibles/Stock Arturo Integrados.xlsx
+++ b/Componentes Disponibles/Stock Arturo Integrados.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="83">
   <si>
     <t>CA3086</t>
   </si>
@@ -186,6 +186,90 @@
   </si>
   <si>
     <t>Cantidad</t>
+  </si>
+  <si>
+    <t>Leds</t>
+  </si>
+  <si>
+    <t>Rojo Cuadrado</t>
+  </si>
+  <si>
+    <t>Rojo 5mm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Blanco 5mm </t>
+  </si>
+  <si>
+    <t>Verde 5mm</t>
+  </si>
+  <si>
+    <t>RGB</t>
+  </si>
+  <si>
+    <t>Amarillo 5mm</t>
+  </si>
+  <si>
+    <t>NE555</t>
+  </si>
+  <si>
+    <t>Clock</t>
+  </si>
+  <si>
+    <t>2.2uf</t>
+  </si>
+  <si>
+    <t>47uf</t>
+  </si>
+  <si>
+    <t>10uf</t>
+  </si>
+  <si>
+    <t>1000uf</t>
+  </si>
+  <si>
+    <t>2200uf</t>
+  </si>
+  <si>
+    <t>47mf</t>
+  </si>
+  <si>
+    <t>470uf</t>
+  </si>
+  <si>
+    <t>0.47uf</t>
+  </si>
+  <si>
+    <t>10n</t>
+  </si>
+  <si>
+    <t>Transistores TO220</t>
+  </si>
+  <si>
+    <t>BC547C</t>
+  </si>
+  <si>
+    <t>BC557</t>
+  </si>
+  <si>
+    <t>C32725</t>
+  </si>
+  <si>
+    <t>LM35</t>
+  </si>
+  <si>
+    <t>IRFZ48N</t>
+  </si>
+  <si>
+    <t>L780 50V</t>
+  </si>
+  <si>
+    <t>LM317T</t>
+  </si>
+  <si>
+    <t>7812CT</t>
+  </si>
+  <si>
+    <t>AN7905ST</t>
   </si>
 </sst>
 </file>
@@ -209,7 +293,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -232,13 +316,28 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -543,15 +642,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A4:J41"/>
+  <dimension ref="A4:Z19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="D41" sqref="D41"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
@@ -563,8 +662,44 @@
       <c r="E4" s="1" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G4" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="M4" s="1"/>
+      <c r="N4" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="P4" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q4" s="1"/>
+      <c r="R4" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="T4" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="U4" s="1"/>
+      <c r="V4" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="X4" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="Y4" s="1"/>
+      <c r="Z4" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>1</v>
       </c>
@@ -576,8 +711,40 @@
       <c r="E5" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G5" s="1"/>
+      <c r="H5" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1">
+        <v>1</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="M5" s="1"/>
+      <c r="N5" s="1">
+        <v>8</v>
+      </c>
+      <c r="P5" s="1"/>
+      <c r="Q5" s="1"/>
+      <c r="R5" s="1"/>
+      <c r="T5" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="U5" s="1"/>
+      <c r="V5" s="1">
+        <v>3</v>
+      </c>
+      <c r="X5" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="Y5" s="1"/>
+      <c r="Z5" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>2</v>
       </c>
@@ -589,8 +756,46 @@
       <c r="E6" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G6" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1">
+        <v>1</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="M6" s="1"/>
+      <c r="N6" s="1">
+        <v>4</v>
+      </c>
+      <c r="P6" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q6" s="1"/>
+      <c r="R6" s="1">
+        <v>5</v>
+      </c>
+      <c r="T6" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="U6" s="1"/>
+      <c r="V6" s="1">
+        <v>1</v>
+      </c>
+      <c r="X6" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="Y6" s="1"/>
+      <c r="Z6" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
@@ -602,8 +807,46 @@
       <c r="E7" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G7" s="1">
+        <v>152</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1">
+        <v>4</v>
+      </c>
+      <c r="L7" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="M7" s="1"/>
+      <c r="N7" s="1">
+        <v>3</v>
+      </c>
+      <c r="P7" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q7" s="1"/>
+      <c r="R7" s="1">
+        <v>1</v>
+      </c>
+      <c r="T7" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="U7" s="1"/>
+      <c r="V7" s="1">
+        <v>1</v>
+      </c>
+      <c r="X7" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="Y7" s="2"/>
+      <c r="Z7" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
@@ -615,8 +858,46 @@
       <c r="E8" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G8" s="1">
+        <v>104</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="I8" s="1"/>
+      <c r="J8" s="1">
+        <v>3</v>
+      </c>
+      <c r="L8" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="M8" s="1"/>
+      <c r="N8" s="1">
+        <v>1</v>
+      </c>
+      <c r="P8" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="Q8" s="1"/>
+      <c r="R8" s="1">
+        <v>7</v>
+      </c>
+      <c r="T8" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="U8" s="1"/>
+      <c r="V8" s="1">
+        <v>1</v>
+      </c>
+      <c r="X8" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="Y8" s="1"/>
+      <c r="Z8" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
@@ -628,8 +909,46 @@
       <c r="E9" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G9" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="I9" s="1"/>
+      <c r="J9" s="1">
+        <v>1</v>
+      </c>
+      <c r="L9" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="M9" s="1"/>
+      <c r="N9" s="3">
+        <v>4</v>
+      </c>
+      <c r="P9" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q9" s="1"/>
+      <c r="R9" s="3">
+        <v>2</v>
+      </c>
+      <c r="T9" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="U9" s="1"/>
+      <c r="V9" s="1">
+        <v>2</v>
+      </c>
+      <c r="X9" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="Y9" s="1"/>
+      <c r="Z9" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>10</v>
       </c>
@@ -641,8 +960,39 @@
       <c r="E10" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G10" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="I10" s="1"/>
+      <c r="J10" s="1">
+        <v>1</v>
+      </c>
+      <c r="L10" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="M10" s="1"/>
+      <c r="N10" s="3">
+        <v>2</v>
+      </c>
+      <c r="P10" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="Q10" s="1"/>
+      <c r="R10" s="3">
+        <v>1</v>
+      </c>
+      <c r="T10" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="U10" s="1"/>
+      <c r="V10" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>12</v>
       </c>
@@ -654,8 +1004,32 @@
       <c r="E11" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G11" s="1">
+        <v>103</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="I11" s="1"/>
+      <c r="J11" s="1">
+        <v>5</v>
+      </c>
+      <c r="L11" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="M11" s="1"/>
+      <c r="N11" s="3">
+        <v>2</v>
+      </c>
+      <c r="P11" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="Q11" s="1"/>
+      <c r="R11" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>13</v>
       </c>
@@ -667,8 +1041,32 @@
       <c r="E12" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G12" s="1">
+        <v>472</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="I12" s="1"/>
+      <c r="J12" s="1">
+        <v>2</v>
+      </c>
+      <c r="L12" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="M12" s="1"/>
+      <c r="N12" s="3">
+        <v>1</v>
+      </c>
+      <c r="P12" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="Q12" s="1"/>
+      <c r="R12" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>15</v>
       </c>
@@ -680,8 +1078,32 @@
       <c r="E13" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G13" s="1">
+        <v>1</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="I13" s="1"/>
+      <c r="J13" s="1">
+        <v>2</v>
+      </c>
+      <c r="L13" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="M13" s="1"/>
+      <c r="N13" s="3">
+        <v>3</v>
+      </c>
+      <c r="P13" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="Q13" s="1"/>
+      <c r="R13" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>16</v>
       </c>
@@ -693,8 +1115,25 @@
       <c r="E14" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G14" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="I14" s="1"/>
+      <c r="J14" s="1">
+        <v>1</v>
+      </c>
+      <c r="L14" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="M14" s="1"/>
+      <c r="N14" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>18</v>
       </c>
@@ -706,8 +1145,25 @@
       <c r="E15" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G15" s="1">
+        <v>47</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="I15" s="1"/>
+      <c r="J15" s="1">
+        <v>1</v>
+      </c>
+      <c r="L15" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="M15" s="1"/>
+      <c r="N15" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>19</v>
       </c>
@@ -719,8 +1175,25 @@
       <c r="E16" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G16" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="I16" s="1"/>
+      <c r="J16" s="1">
+        <v>1</v>
+      </c>
+      <c r="L16" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="M16" s="1"/>
+      <c r="N16" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>21</v>
       </c>
@@ -732,8 +1205,25 @@
       <c r="E17" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G17" s="1">
+        <v>100</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="I17" s="1"/>
+      <c r="J17" s="1">
+        <v>4</v>
+      </c>
+      <c r="L17" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="M17" s="1"/>
+      <c r="N17" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>25</v>
       </c>
@@ -745,257 +1235,38 @@
       <c r="E18" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B20" s="1"/>
-      <c r="C20" s="1"/>
-      <c r="D20" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A21" s="1"/>
-      <c r="B21" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C21" s="1"/>
-      <c r="D21" s="1">
-        <v>1</v>
-      </c>
-      <c r="H21" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="I21" s="1"/>
-      <c r="J21" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C22" s="1"/>
-      <c r="D22" s="1">
-        <v>1</v>
-      </c>
-      <c r="H22" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="I22" s="1"/>
-      <c r="J22" s="1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A23" s="1">
-        <v>152</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C23" s="1"/>
-      <c r="D23" s="1">
-        <v>4</v>
-      </c>
-      <c r="H23" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="I23" s="1"/>
-      <c r="J23" s="1">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A24" s="1">
-        <v>104</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C24" s="1"/>
-      <c r="D24" s="1">
+      <c r="G18" s="1">
+        <v>224</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="I18" s="1"/>
+      <c r="J18" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="3">
+        <v>1</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="H19" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="I19" s="1"/>
+      <c r="J19" s="3">
         <v>2</v>
-      </c>
-      <c r="H24" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="I24" s="1"/>
-      <c r="J24" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A25" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C25" s="1"/>
-      <c r="D25" s="1">
-        <v>1</v>
-      </c>
-      <c r="H25" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="I25" s="1"/>
-      <c r="J25" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A26" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="C26" s="1"/>
-      <c r="D26" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A27" s="1">
-        <v>103</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="C27" s="1"/>
-      <c r="D27" s="1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A28" s="1">
-        <v>472</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="C28" s="1"/>
-      <c r="D28" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A29" s="1">
-        <v>1</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="C29" s="1"/>
-      <c r="D29" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A30" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="C30" s="1"/>
-      <c r="D30" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A31" s="1">
-        <v>47</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="C31" s="1"/>
-      <c r="D31" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A32" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C32" s="1"/>
-      <c r="D32" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="1">
-        <v>100</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="C33" s="1"/>
-      <c r="D33" s="1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="1">
-        <v>224</v>
-      </c>
-      <c r="B34" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="C34" s="1"/>
-      <c r="D34" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="B37" s="1"/>
-      <c r="C37" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="1"/>
-      <c r="B38" s="1"/>
-      <c r="C38" s="1"/>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="B39" s="1"/>
-      <c r="C39" s="1">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="B40" s="1"/>
-      <c r="C40" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="B41" s="1"/>
-      <c r="C41" s="1">
-        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>